<commit_message>
fix(import): add missing resolveClientOptionValues method to ImportController
</commit_message>
<xml_diff>
--- a/Access_Data_Export/clients.xlsx
+++ b/Access_Data_Export/clients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Claude\Litigation_Database_Ver2\Litigation_Database_Ver2\Access_Data_Export\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E32A0952-A0EC-455D-A620-E01356934625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F164B705-E121-4706-8FB2-2DA1F18F4EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2017,18 +2017,6 @@
     <t>Hamada Kamal Ahmed (2)</t>
   </si>
   <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>cash_or_probono</t>
-  </si>
-  <si>
-    <t>power_of_attorney_location</t>
-  </si>
-  <si>
-    <t>documents_location</t>
-  </si>
-  <si>
     <t>contact_lawyer</t>
   </si>
   <si>
@@ -2048,6 +2036,18 @@
   </si>
   <si>
     <t>client_end</t>
+  </si>
+  <si>
+    <t>status_id</t>
+  </si>
+  <si>
+    <t>cash_or_probono_id</t>
+  </si>
+  <si>
+    <t>power_of_attorney_location_id</t>
+  </si>
+  <si>
+    <t>documents_location_id</t>
   </si>
 </sst>
 </file>
@@ -2122,11 +2122,11 @@
     <tableColumn id="2" xr3:uid="{CAE2ADCD-48CF-4EDF-8E9F-08E60057D81C}" name="client_name_en"/>
     <tableColumn id="3" xr3:uid="{0A07B822-AC5E-4702-8E32-C3E83C2C4476}" name="client_print_name"/>
     <tableColumn id="4" xr3:uid="{C7BA75FD-47C5-498D-8710-DD906D97334E}" name="client_name_ar"/>
-    <tableColumn id="5" xr3:uid="{365DB2B1-EABF-46A5-8156-35F2C05C6469}" name="cash_or_probono"/>
-    <tableColumn id="6" xr3:uid="{A3D98335-5976-434F-996D-F08F448AF643}" name="status"/>
+    <tableColumn id="5" xr3:uid="{365DB2B1-EABF-46A5-8156-35F2C05C6469}" name="cash_or_probono_id"/>
+    <tableColumn id="6" xr3:uid="{A3D98335-5976-434F-996D-F08F448AF643}" name="status_id"/>
     <tableColumn id="7" xr3:uid="{AD7FDB29-825C-4F7A-993A-BDC11D0CE0D5}" name="logo"/>
-    <tableColumn id="8" xr3:uid="{E0FBF4B6-3E9B-423D-B3B5-1A8E4C7D09F8}" name="power_of_attorney_location"/>
-    <tableColumn id="9" xr3:uid="{20F3D9A5-4509-4787-84F8-5428D6553654}" name="documents_location"/>
+    <tableColumn id="8" xr3:uid="{E0FBF4B6-3E9B-423D-B3B5-1A8E4C7D09F8}" name="power_of_attorney_location_id"/>
+    <tableColumn id="9" xr3:uid="{20F3D9A5-4509-4787-84F8-5428D6553654}" name="documents_location_id"/>
     <tableColumn id="10" xr3:uid="{FFBB3084-AC24-4F58-8EFD-2417F7F83D34}" name="contact_lawyer"/>
     <tableColumn id="14" xr3:uid="{BC354857-7A23-46C6-ADFA-0D81BC38781A}" name="lawyer_id"/>
     <tableColumn id="11" xr3:uid="{027BD1CA-7803-4AC0-A969-2F1DD8D63C41}" name="client_start" dataDxfId="0"/>
@@ -2426,7 +2426,7 @@
   <dimension ref="A1:M309"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I1" sqref="H1:I1048576"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2447,43 +2447,43 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="B1" t="s">
+        <v>663</v>
+      </c>
+      <c r="C1" t="s">
+        <v>664</v>
+      </c>
+      <c r="D1" t="s">
+        <v>662</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>668</v>
+      </c>
+      <c r="F1" t="s">
         <v>667</v>
-      </c>
-      <c r="C1" t="s">
-        <v>668</v>
-      </c>
-      <c r="D1" t="s">
-        <v>666</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>661</v>
-      </c>
-      <c r="F1" t="s">
-        <v>660</v>
       </c>
       <c r="G1" t="s">
         <v>0</v>
       </c>
       <c r="H1" t="s">
-        <v>662</v>
+        <v>669</v>
       </c>
       <c r="I1" t="s">
-        <v>663</v>
+        <v>670</v>
       </c>
       <c r="J1" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="K1" t="s">
         <v>657</v>
       </c>
       <c r="L1" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
       <c r="M1" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
@@ -2503,10 +2503,10 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J2" t="s">
         <v>658</v>
@@ -2535,10 +2535,10 @@
         <v>1</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J3" t="s">
         <v>658</v>
@@ -2567,10 +2567,10 @@
         <v>1</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J4" t="s">
         <v>658</v>
@@ -2596,10 +2596,10 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J5" t="s">
         <v>658</v>
@@ -2628,10 +2628,10 @@
         <v>1</v>
       </c>
       <c r="F6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J6" t="s">
         <v>658</v>
@@ -2660,10 +2660,10 @@
         <v>1</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J7" t="s">
         <v>658</v>
@@ -2692,10 +2692,10 @@
         <v>1</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J8" t="s">
         <v>658</v>
@@ -2724,10 +2724,10 @@
         <v>3</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J9" t="s">
         <v>658</v>
@@ -2753,10 +2753,10 @@
         <v>3</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J10" t="s">
         <v>658</v>
@@ -2782,10 +2782,10 @@
         <v>1</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J11" t="s">
         <v>658</v>
@@ -2811,10 +2811,10 @@
         <v>1</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H12">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J12" t="s">
         <v>658</v>
@@ -2840,10 +2840,10 @@
         <v>1</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H13">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J13" t="s">
         <v>658</v>
@@ -2869,10 +2869,10 @@
         <v>1</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J14" t="s">
         <v>658</v>
@@ -2898,10 +2898,10 @@
         <v>1</v>
       </c>
       <c r="F15">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H15">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J15" t="s">
         <v>658</v>
@@ -2927,10 +2927,10 @@
         <v>1</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H16">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J16" t="s">
         <v>658</v>
@@ -2956,10 +2956,10 @@
         <v>2</v>
       </c>
       <c r="F17">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H17">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J17" t="s">
         <v>658</v>
@@ -2985,10 +2985,10 @@
         <v>1</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H18">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J18" t="s">
         <v>658</v>
@@ -3014,13 +3014,13 @@
         <v>1</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H19">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I19">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J19" t="s">
         <v>658</v>
@@ -3046,10 +3046,10 @@
         <v>2</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H20">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J20" t="s">
         <v>658</v>
@@ -3075,10 +3075,10 @@
         <v>1</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H21">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J21" t="s">
         <v>658</v>
@@ -3104,10 +3104,10 @@
         <v>1</v>
       </c>
       <c r="F22">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H22">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J22" t="s">
         <v>658</v>
@@ -3133,10 +3133,10 @@
         <v>1</v>
       </c>
       <c r="F23">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H23">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J23" t="s">
         <v>658</v>
@@ -3162,10 +3162,10 @@
         <v>1</v>
       </c>
       <c r="F24">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H24">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J24" t="s">
         <v>658</v>
@@ -3191,10 +3191,10 @@
         <v>1</v>
       </c>
       <c r="F25">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H25">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J25" t="s">
         <v>658</v>
@@ -3220,10 +3220,10 @@
         <v>1</v>
       </c>
       <c r="F26">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H26">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J26" t="s">
         <v>658</v>
@@ -3249,10 +3249,10 @@
         <v>1</v>
       </c>
       <c r="F27">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H27">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J27" t="s">
         <v>658</v>
@@ -3278,10 +3278,10 @@
         <v>1</v>
       </c>
       <c r="F28">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H28">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J28" t="s">
         <v>658</v>
@@ -3307,10 +3307,10 @@
         <v>1</v>
       </c>
       <c r="F29">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H29">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J29" t="s">
         <v>658</v>
@@ -3336,10 +3336,10 @@
         <v>1</v>
       </c>
       <c r="F30">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H30">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J30" t="s">
         <v>658</v>
@@ -3365,10 +3365,10 @@
         <v>1</v>
       </c>
       <c r="F31">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H31">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J31" t="s">
         <v>658</v>
@@ -3394,10 +3394,10 @@
         <v>1</v>
       </c>
       <c r="F32">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H32">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J32" t="s">
         <v>658</v>
@@ -3423,13 +3423,13 @@
         <v>1</v>
       </c>
       <c r="F33">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G33" t="s">
         <v>118</v>
       </c>
       <c r="H33">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J33" t="s">
         <v>658</v>
@@ -3455,10 +3455,10 @@
         <v>1</v>
       </c>
       <c r="F34">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H34">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J34" t="s">
         <v>658</v>
@@ -3484,10 +3484,10 @@
         <v>1</v>
       </c>
       <c r="F35">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H35">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J35" t="s">
         <v>658</v>
@@ -3513,13 +3513,13 @@
         <v>1</v>
       </c>
       <c r="F36">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G36" t="s">
         <v>125</v>
       </c>
       <c r="H36">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J36" t="s">
         <v>658</v>
@@ -3545,10 +3545,10 @@
         <v>1</v>
       </c>
       <c r="F37">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H37">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J37" t="s">
         <v>658</v>
@@ -3574,10 +3574,10 @@
         <v>1</v>
       </c>
       <c r="F38">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H38">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J38" t="s">
         <v>658</v>
@@ -3603,10 +3603,10 @@
         <v>1</v>
       </c>
       <c r="F39">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H39">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J39" t="s">
         <v>658</v>
@@ -3632,10 +3632,10 @@
         <v>1</v>
       </c>
       <c r="F40">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H40">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J40" t="s">
         <v>658</v>
@@ -3661,10 +3661,10 @@
         <v>1</v>
       </c>
       <c r="F41">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H41">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J41" t="s">
         <v>658</v>
@@ -3690,10 +3690,10 @@
         <v>1</v>
       </c>
       <c r="F42">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H42">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="J42" t="s">
         <v>658</v>
@@ -3719,10 +3719,10 @@
         <v>1</v>
       </c>
       <c r="F43">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H43">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J43" t="s">
         <v>658</v>
@@ -3748,10 +3748,10 @@
         <v>1</v>
       </c>
       <c r="F44">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H44">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J44" t="s">
         <v>658</v>
@@ -3777,10 +3777,10 @@
         <v>1</v>
       </c>
       <c r="F45">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H45">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J45" t="s">
         <v>658</v>
@@ -3806,10 +3806,10 @@
         <v>1</v>
       </c>
       <c r="F46">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H46">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J46" t="s">
         <v>658</v>
@@ -3835,10 +3835,10 @@
         <v>1</v>
       </c>
       <c r="F47">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H47">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J47" t="s">
         <v>658</v>
@@ -3864,10 +3864,10 @@
         <v>1</v>
       </c>
       <c r="F48">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H48">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J48" t="s">
         <v>658</v>
@@ -3893,10 +3893,10 @@
         <v>1</v>
       </c>
       <c r="F49">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H49">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J49" t="s">
         <v>658</v>
@@ -3922,10 +3922,10 @@
         <v>1</v>
       </c>
       <c r="F50">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H50">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J50" t="s">
         <v>658</v>
@@ -3951,10 +3951,10 @@
         <v>1</v>
       </c>
       <c r="F51">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H51">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J51" t="s">
         <v>658</v>
@@ -3980,10 +3980,10 @@
         <v>1</v>
       </c>
       <c r="F52">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H52">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J52" t="s">
         <v>658</v>
@@ -4009,10 +4009,10 @@
         <v>1</v>
       </c>
       <c r="F53">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H53">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J53" t="s">
         <v>658</v>
@@ -4038,10 +4038,10 @@
         <v>1</v>
       </c>
       <c r="F54">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H54">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J54" t="s">
         <v>658</v>
@@ -4067,10 +4067,10 @@
         <v>1</v>
       </c>
       <c r="F55">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H55">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J55" t="s">
         <v>658</v>
@@ -4096,10 +4096,10 @@
         <v>1</v>
       </c>
       <c r="F56">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H56">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J56" t="s">
         <v>658</v>
@@ -4125,10 +4125,10 @@
         <v>1</v>
       </c>
       <c r="F57">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H57">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J57" t="s">
         <v>658</v>
@@ -4154,10 +4154,10 @@
         <v>2</v>
       </c>
       <c r="F58">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H58">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="J58" t="s">
         <v>658</v>
@@ -4183,10 +4183,10 @@
         <v>1</v>
       </c>
       <c r="F59">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H59">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J59" t="s">
         <v>658</v>
@@ -4212,10 +4212,10 @@
         <v>1</v>
       </c>
       <c r="F60">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H60">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J60" t="s">
         <v>658</v>
@@ -4241,10 +4241,10 @@
         <v>1</v>
       </c>
       <c r="F61">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H61">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J61" t="s">
         <v>658</v>
@@ -4270,10 +4270,10 @@
         <v>1</v>
       </c>
       <c r="F62">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H62">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J62" t="s">
         <v>658</v>
@@ -4299,10 +4299,10 @@
         <v>1</v>
       </c>
       <c r="F63">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H63">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J63" t="s">
         <v>658</v>
@@ -4328,10 +4328,10 @@
         <v>1</v>
       </c>
       <c r="F64">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H64">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J64" t="s">
         <v>658</v>
@@ -4357,10 +4357,10 @@
         <v>1</v>
       </c>
       <c r="F65">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H65">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J65" t="s">
         <v>658</v>
@@ -4386,10 +4386,10 @@
         <v>1</v>
       </c>
       <c r="F66">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H66">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J66" t="s">
         <v>658</v>
@@ -4415,10 +4415,10 @@
         <v>1</v>
       </c>
       <c r="F67">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H67">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="J67" t="s">
         <v>658</v>
@@ -4444,10 +4444,10 @@
         <v>1</v>
       </c>
       <c r="F68">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H68">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J68" t="s">
         <v>658</v>
@@ -4473,10 +4473,10 @@
         <v>1</v>
       </c>
       <c r="F69">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H69">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J69" t="s">
         <v>658</v>
@@ -4502,10 +4502,10 @@
         <v>1</v>
       </c>
       <c r="F70">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H70">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J70" t="s">
         <v>658</v>
@@ -4531,10 +4531,10 @@
         <v>1</v>
       </c>
       <c r="F71">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H71">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J71" t="s">
         <v>658</v>
@@ -4560,10 +4560,10 @@
         <v>1</v>
       </c>
       <c r="F72">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H72">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J72" t="s">
         <v>658</v>
@@ -4589,10 +4589,10 @@
         <v>1</v>
       </c>
       <c r="F73">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H73">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J73" t="s">
         <v>658</v>
@@ -4618,10 +4618,10 @@
         <v>1</v>
       </c>
       <c r="F74">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H74">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J74" t="s">
         <v>658</v>
@@ -4647,10 +4647,10 @@
         <v>1</v>
       </c>
       <c r="F75">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H75">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J75" t="s">
         <v>658</v>
@@ -4676,13 +4676,13 @@
         <v>1</v>
       </c>
       <c r="F76">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G76" t="s">
         <v>194</v>
       </c>
       <c r="H76">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J76" t="s">
         <v>658</v>
@@ -4708,10 +4708,10 @@
         <v>1</v>
       </c>
       <c r="F77">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H77">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J77" t="s">
         <v>658</v>
@@ -4737,10 +4737,10 @@
         <v>1</v>
       </c>
       <c r="F78">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H78">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J78" t="s">
         <v>658</v>
@@ -4766,10 +4766,10 @@
         <v>1</v>
       </c>
       <c r="F79">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H79">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J79" t="s">
         <v>658</v>
@@ -4795,10 +4795,10 @@
         <v>1</v>
       </c>
       <c r="F80">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H80">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J80" t="s">
         <v>658</v>
@@ -4824,10 +4824,10 @@
         <v>1</v>
       </c>
       <c r="F81">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H81">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J81" t="s">
         <v>658</v>
@@ -4853,10 +4853,10 @@
         <v>1</v>
       </c>
       <c r="F82">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H82">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J82" t="s">
         <v>658</v>
@@ -4882,10 +4882,10 @@
         <v>2</v>
       </c>
       <c r="F83">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H83">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J83" t="s">
         <v>658</v>
@@ -4911,10 +4911,10 @@
         <v>1</v>
       </c>
       <c r="F84">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H84">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J84" t="s">
         <v>658</v>
@@ -4940,10 +4940,10 @@
         <v>1</v>
       </c>
       <c r="F85">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H85">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J85" t="s">
         <v>658</v>
@@ -4969,10 +4969,10 @@
         <v>1</v>
       </c>
       <c r="F86">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H86">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J86" t="s">
         <v>658</v>
@@ -4998,10 +4998,10 @@
         <v>1</v>
       </c>
       <c r="F87">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H87">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J87" t="s">
         <v>658</v>
@@ -5027,10 +5027,10 @@
         <v>1</v>
       </c>
       <c r="F88">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H88">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J88" t="s">
         <v>658</v>
@@ -5056,10 +5056,10 @@
         <v>1</v>
       </c>
       <c r="F89">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H89">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J89" t="s">
         <v>658</v>
@@ -5085,10 +5085,10 @@
         <v>1</v>
       </c>
       <c r="F90">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H90">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J90" t="s">
         <v>658</v>
@@ -5114,10 +5114,10 @@
         <v>1</v>
       </c>
       <c r="F91">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H91">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J91" t="s">
         <v>658</v>
@@ -5143,10 +5143,10 @@
         <v>1</v>
       </c>
       <c r="F92">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H92">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J92" t="s">
         <v>658</v>
@@ -5172,10 +5172,10 @@
         <v>1</v>
       </c>
       <c r="F93">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H93">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J93" t="s">
         <v>658</v>
@@ -5201,10 +5201,10 @@
         <v>1</v>
       </c>
       <c r="F94">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H94">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J94" t="s">
         <v>658</v>
@@ -5230,10 +5230,10 @@
         <v>1</v>
       </c>
       <c r="F95">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H95">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J95" t="s">
         <v>658</v>
@@ -5259,13 +5259,13 @@
         <v>2</v>
       </c>
       <c r="F96">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G96" t="s">
         <v>260</v>
       </c>
       <c r="H96">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J96" t="s">
         <v>658</v>
@@ -5291,10 +5291,10 @@
         <v>1</v>
       </c>
       <c r="F97">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H97">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J97" t="s">
         <v>658</v>
@@ -5320,10 +5320,10 @@
         <v>1</v>
       </c>
       <c r="F98">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H98">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J98" t="s">
         <v>658</v>
@@ -5349,10 +5349,10 @@
         <v>1</v>
       </c>
       <c r="F99">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H99">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J99" t="s">
         <v>658</v>
@@ -5378,10 +5378,10 @@
         <v>1</v>
       </c>
       <c r="F100">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H100">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J100" t="s">
         <v>658</v>
@@ -5407,10 +5407,10 @@
         <v>2</v>
       </c>
       <c r="F101">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H101">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J101" t="s">
         <v>658</v>
@@ -5436,10 +5436,10 @@
         <v>1</v>
       </c>
       <c r="F102">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H102">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J102" t="s">
         <v>658</v>
@@ -5465,10 +5465,10 @@
         <v>1</v>
       </c>
       <c r="F103">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H103">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J103" t="s">
         <v>658</v>
@@ -5494,10 +5494,10 @@
         <v>1</v>
       </c>
       <c r="F104">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H104">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J104" t="s">
         <v>658</v>
@@ -5523,10 +5523,10 @@
         <v>1</v>
       </c>
       <c r="F105">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H105">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J105" t="s">
         <v>658</v>
@@ -5552,10 +5552,10 @@
         <v>1</v>
       </c>
       <c r="F106">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H106">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J106" t="s">
         <v>658</v>
@@ -5581,10 +5581,10 @@
         <v>1</v>
       </c>
       <c r="F107">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H107">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J107" t="s">
         <v>658</v>
@@ -5610,10 +5610,10 @@
         <v>1</v>
       </c>
       <c r="F108">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H108">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="J108" t="s">
         <v>658</v>
@@ -5639,13 +5639,13 @@
         <v>1</v>
       </c>
       <c r="F109">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H109">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I109">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J109" t="s">
         <v>658</v>
@@ -5671,10 +5671,10 @@
         <v>2</v>
       </c>
       <c r="F110">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H110">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J110" t="s">
         <v>658</v>
@@ -5700,13 +5700,13 @@
         <v>1</v>
       </c>
       <c r="F111">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H111">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I111">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J111" t="s">
         <v>658</v>
@@ -5732,13 +5732,13 @@
         <v>2</v>
       </c>
       <c r="F112">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H112">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I112">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J112" t="s">
         <v>658</v>
@@ -5764,10 +5764,10 @@
         <v>2</v>
       </c>
       <c r="F113">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H113">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J113" t="s">
         <v>658</v>
@@ -5793,10 +5793,10 @@
         <v>1</v>
       </c>
       <c r="F114">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H114">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J114" t="s">
         <v>658</v>
@@ -5822,10 +5822,10 @@
         <v>1</v>
       </c>
       <c r="F115">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H115">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J115" t="s">
         <v>658</v>
@@ -5851,10 +5851,10 @@
         <v>1</v>
       </c>
       <c r="F116">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H116">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J116" t="s">
         <v>658</v>
@@ -5880,10 +5880,10 @@
         <v>1</v>
       </c>
       <c r="F117">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H117">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J117" t="s">
         <v>658</v>
@@ -5909,10 +5909,10 @@
         <v>1</v>
       </c>
       <c r="F118">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H118">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J118" t="s">
         <v>658</v>
@@ -5938,10 +5938,10 @@
         <v>1</v>
       </c>
       <c r="F119">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H119">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J119" t="s">
         <v>658</v>
@@ -5967,10 +5967,10 @@
         <v>1</v>
       </c>
       <c r="F120">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H120">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J120" t="s">
         <v>658</v>
@@ -5996,10 +5996,10 @@
         <v>1</v>
       </c>
       <c r="F121">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H121">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J121" t="s">
         <v>658</v>
@@ -6025,10 +6025,10 @@
         <v>1</v>
       </c>
       <c r="F122">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H122">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J122" t="s">
         <v>658</v>
@@ -6054,10 +6054,10 @@
         <v>1</v>
       </c>
       <c r="F123">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H123">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J123" t="s">
         <v>658</v>
@@ -6083,10 +6083,10 @@
         <v>1</v>
       </c>
       <c r="F124">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H124">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J124" t="s">
         <v>658</v>
@@ -6112,10 +6112,10 @@
         <v>1</v>
       </c>
       <c r="F125">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H125">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J125" t="s">
         <v>658</v>
@@ -6141,13 +6141,13 @@
         <v>1</v>
       </c>
       <c r="F126">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G126" t="s">
         <v>312</v>
       </c>
       <c r="H126">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J126" t="s">
         <v>658</v>
@@ -6173,13 +6173,13 @@
         <v>1</v>
       </c>
       <c r="F127">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G127" t="s">
         <v>316</v>
       </c>
       <c r="H127">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J127" t="s">
         <v>658</v>
@@ -6205,10 +6205,10 @@
         <v>1</v>
       </c>
       <c r="F128">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H128">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J128" t="s">
         <v>658</v>
@@ -6234,10 +6234,10 @@
         <v>1</v>
       </c>
       <c r="F129">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H129">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J129" t="s">
         <v>658</v>
@@ -6263,10 +6263,10 @@
         <v>1</v>
       </c>
       <c r="F130">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H130">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J130" t="s">
         <v>658</v>
@@ -6292,10 +6292,10 @@
         <v>1</v>
       </c>
       <c r="F131">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H131">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J131" t="s">
         <v>658</v>
@@ -6321,10 +6321,10 @@
         <v>1</v>
       </c>
       <c r="F132">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H132">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J132" t="s">
         <v>658</v>
@@ -6350,10 +6350,10 @@
         <v>1</v>
       </c>
       <c r="F133">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H133">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J133" t="s">
         <v>658</v>
@@ -6379,10 +6379,10 @@
         <v>1</v>
       </c>
       <c r="F134">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H134">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J134" t="s">
         <v>658</v>
@@ -6408,10 +6408,10 @@
         <v>1</v>
       </c>
       <c r="F135">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H135">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J135" t="s">
         <v>658</v>
@@ -6437,10 +6437,10 @@
         <v>1</v>
       </c>
       <c r="F136">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H136">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J136" t="s">
         <v>658</v>
@@ -6466,10 +6466,10 @@
         <v>1</v>
       </c>
       <c r="F137">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H137">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J137" t="s">
         <v>658</v>
@@ -6495,10 +6495,10 @@
         <v>1</v>
       </c>
       <c r="F138">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H138">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J138" t="s">
         <v>658</v>
@@ -6524,10 +6524,10 @@
         <v>2</v>
       </c>
       <c r="F139">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H139">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J139" t="s">
         <v>658</v>
@@ -6553,13 +6553,13 @@
         <v>1</v>
       </c>
       <c r="F140">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G140" t="s">
         <v>350</v>
       </c>
       <c r="H140">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J140" t="s">
         <v>658</v>
@@ -6585,16 +6585,16 @@
         <v>1</v>
       </c>
       <c r="F141">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G141" t="s">
         <v>353</v>
       </c>
       <c r="H141">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I141">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J141" t="s">
         <v>658</v>
@@ -6620,10 +6620,10 @@
         <v>1</v>
       </c>
       <c r="F142">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H142">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J142" t="s">
         <v>658</v>
@@ -6649,10 +6649,10 @@
         <v>2</v>
       </c>
       <c r="F143">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H143">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J143" t="s">
         <v>658</v>
@@ -6678,10 +6678,10 @@
         <v>1</v>
       </c>
       <c r="F144">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H144">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J144" t="s">
         <v>658</v>
@@ -6707,13 +6707,13 @@
         <v>1</v>
       </c>
       <c r="F145">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G145" t="s">
         <v>368</v>
       </c>
       <c r="H145">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J145" t="s">
         <v>658</v>
@@ -6739,10 +6739,10 @@
         <v>2</v>
       </c>
       <c r="F146">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H146">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J146" t="s">
         <v>658</v>
@@ -6768,13 +6768,13 @@
         <v>2</v>
       </c>
       <c r="F147">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G147" t="s">
         <v>377</v>
       </c>
       <c r="H147">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J147" t="s">
         <v>658</v>
@@ -6800,10 +6800,10 @@
         <v>1</v>
       </c>
       <c r="F148">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H148">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J148" t="s">
         <v>658</v>
@@ -6829,10 +6829,10 @@
         <v>1</v>
       </c>
       <c r="F149">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H149">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J149" t="s">
         <v>658</v>
@@ -6858,10 +6858,10 @@
         <v>1</v>
       </c>
       <c r="F150">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H150">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J150" t="s">
         <v>658</v>
@@ -6887,10 +6887,10 @@
         <v>2</v>
       </c>
       <c r="F151">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H151">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J151" t="s">
         <v>658</v>
@@ -6916,10 +6916,10 @@
         <v>1</v>
       </c>
       <c r="F152">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H152">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J152" t="s">
         <v>658</v>
@@ -6945,10 +6945,10 @@
         <v>1</v>
       </c>
       <c r="F153">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H153">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J153" t="s">
         <v>658</v>
@@ -6974,10 +6974,10 @@
         <v>2</v>
       </c>
       <c r="F154">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H154">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J154" t="s">
         <v>658</v>
@@ -7003,10 +7003,10 @@
         <v>1</v>
       </c>
       <c r="F155">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H155">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J155" t="s">
         <v>658</v>
@@ -7032,13 +7032,13 @@
         <v>1</v>
       </c>
       <c r="F156">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G156" t="s">
         <v>394</v>
       </c>
       <c r="H156">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J156" t="s">
         <v>658</v>
@@ -7064,10 +7064,10 @@
         <v>1</v>
       </c>
       <c r="F157">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H157">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J157" t="s">
         <v>658</v>
@@ -7093,10 +7093,10 @@
         <v>1</v>
       </c>
       <c r="F158">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H158">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J158" t="s">
         <v>658</v>
@@ -7122,10 +7122,10 @@
         <v>1</v>
       </c>
       <c r="F159">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H159">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J159" t="s">
         <v>658</v>
@@ -7151,10 +7151,10 @@
         <v>1</v>
       </c>
       <c r="F160">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H160">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J160" t="s">
         <v>658</v>
@@ -7180,10 +7180,10 @@
         <v>1</v>
       </c>
       <c r="F161">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H161">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J161" t="s">
         <v>658</v>
@@ -7209,10 +7209,10 @@
         <v>1</v>
       </c>
       <c r="F162">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H162">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J162" t="s">
         <v>658</v>
@@ -7238,10 +7238,10 @@
         <v>1</v>
       </c>
       <c r="F163">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H163">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J163" t="s">
         <v>658</v>
@@ -7267,10 +7267,10 @@
         <v>1</v>
       </c>
       <c r="F164">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H164">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J164" t="s">
         <v>658</v>
@@ -7296,13 +7296,13 @@
         <v>1</v>
       </c>
       <c r="F165">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G165" t="s">
         <v>433</v>
       </c>
       <c r="H165">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J165" t="s">
         <v>658</v>
@@ -7328,13 +7328,13 @@
         <v>1</v>
       </c>
       <c r="F166">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G166" t="s">
         <v>437</v>
       </c>
       <c r="H166">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J166" t="s">
         <v>658</v>
@@ -7360,10 +7360,10 @@
         <v>2</v>
       </c>
       <c r="F167">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H167">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J167" t="s">
         <v>658</v>
@@ -7389,10 +7389,10 @@
         <v>1</v>
       </c>
       <c r="F168">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H168">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J168" t="s">
         <v>658</v>
@@ -7418,10 +7418,10 @@
         <v>1</v>
       </c>
       <c r="F169">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H169">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J169" t="s">
         <v>658</v>
@@ -7447,10 +7447,10 @@
         <v>1</v>
       </c>
       <c r="F170">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H170">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J170" t="s">
         <v>658</v>
@@ -7476,10 +7476,10 @@
         <v>1</v>
       </c>
       <c r="F171">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H171">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J171" t="s">
         <v>658</v>
@@ -7505,13 +7505,13 @@
         <v>1</v>
       </c>
       <c r="F172">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G172" t="s">
         <v>458</v>
       </c>
       <c r="H172">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J172" t="s">
         <v>658</v>
@@ -7540,13 +7540,13 @@
         <v>1</v>
       </c>
       <c r="F173">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G173" t="s">
         <v>461</v>
       </c>
       <c r="H173">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J173" t="s">
         <v>658</v>
@@ -7572,10 +7572,10 @@
         <v>2</v>
       </c>
       <c r="F174">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H174">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J174" t="s">
         <v>658</v>
@@ -7604,13 +7604,13 @@
         <v>1</v>
       </c>
       <c r="F175">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G175" t="s">
         <v>484</v>
       </c>
       <c r="H175">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J175" t="s">
         <v>658</v>
@@ -7636,10 +7636,10 @@
         <v>1</v>
       </c>
       <c r="F176">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H176">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J176" t="s">
         <v>658</v>
@@ -7665,10 +7665,10 @@
         <v>2</v>
       </c>
       <c r="F177">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H177">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J177" t="s">
         <v>658</v>
@@ -7697,13 +7697,13 @@
         <v>1</v>
       </c>
       <c r="F178">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G178" t="s">
         <v>507</v>
       </c>
       <c r="H178">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J178" t="s">
         <v>658</v>
@@ -7732,10 +7732,10 @@
         <v>2</v>
       </c>
       <c r="F179">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H179">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J179" t="s">
         <v>658</v>
@@ -7764,10 +7764,10 @@
         <v>2</v>
       </c>
       <c r="F180">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H180">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J180" t="s">
         <v>658</v>
@@ -7796,10 +7796,10 @@
         <v>1</v>
       </c>
       <c r="F181">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H181">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J181" t="s">
         <v>658</v>
@@ -7825,10 +7825,10 @@
         <v>1</v>
       </c>
       <c r="F182">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H182">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J182" t="s">
         <v>658</v>
@@ -7854,10 +7854,10 @@
         <v>1</v>
       </c>
       <c r="F183">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H183">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J183" t="s">
         <v>658</v>
@@ -7889,10 +7889,10 @@
         <v>1</v>
       </c>
       <c r="F184">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H184">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J184" t="s">
         <v>658</v>
@@ -7921,10 +7921,10 @@
         <v>1</v>
       </c>
       <c r="F185">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H185">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J185" t="s">
         <v>658</v>
@@ -7953,10 +7953,10 @@
         <v>1</v>
       </c>
       <c r="F186">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H186">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J186" t="s">
         <v>658</v>
@@ -7985,10 +7985,10 @@
         <v>2</v>
       </c>
       <c r="F187">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H187">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J187" t="s">
         <v>658</v>
@@ -8017,10 +8017,10 @@
         <v>1</v>
       </c>
       <c r="F188">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H188">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J188" t="s">
         <v>658</v>
@@ -8049,10 +8049,10 @@
         <v>1</v>
       </c>
       <c r="F189">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H189">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J189" t="s">
         <v>658</v>
@@ -8081,13 +8081,13 @@
         <v>1</v>
       </c>
       <c r="F190">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H190">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I190">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="J190" t="s">
         <v>658</v>
@@ -8116,10 +8116,10 @@
         <v>1</v>
       </c>
       <c r="F191">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H191">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J191" t="s">
         <v>658</v>
@@ -8148,10 +8148,10 @@
         <v>1</v>
       </c>
       <c r="F192">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H192">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J192" t="s">
         <v>658</v>
@@ -8180,10 +8180,10 @@
         <v>2</v>
       </c>
       <c r="F193">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H193">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J193" t="s">
         <v>658</v>
@@ -8212,10 +8212,10 @@
         <v>1</v>
       </c>
       <c r="F194">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H194">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J194" t="s">
         <v>658</v>
@@ -8244,10 +8244,10 @@
         <v>1</v>
       </c>
       <c r="F195">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H195">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J195" t="s">
         <v>658</v>
@@ -8276,13 +8276,13 @@
         <v>1</v>
       </c>
       <c r="F196">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G196" t="s">
         <v>54</v>
       </c>
       <c r="H196">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J196" t="s">
         <v>55</v>
@@ -8308,10 +8308,10 @@
         <v>1</v>
       </c>
       <c r="F197">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H197">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J197" t="s">
         <v>55</v>
@@ -8337,10 +8337,10 @@
         <v>1</v>
       </c>
       <c r="F198">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H198">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J198" t="s">
         <v>55</v>
@@ -8366,10 +8366,10 @@
         <v>1</v>
       </c>
       <c r="F199">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H199">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J199" t="s">
         <v>55</v>
@@ -8395,10 +8395,10 @@
         <v>1</v>
       </c>
       <c r="F200">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H200">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J200" t="s">
         <v>55</v>
@@ -8424,13 +8424,13 @@
         <v>1</v>
       </c>
       <c r="F201">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G201" t="s">
         <v>221</v>
       </c>
       <c r="H201">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J201" t="s">
         <v>55</v>
@@ -8456,10 +8456,10 @@
         <v>1</v>
       </c>
       <c r="F202">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H202">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J202" t="s">
         <v>55</v>
@@ -8485,10 +8485,10 @@
         <v>2</v>
       </c>
       <c r="F203">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H203">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J203" t="s">
         <v>55</v>
@@ -8514,13 +8514,13 @@
         <v>1</v>
       </c>
       <c r="F204">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G204" t="s">
         <v>247</v>
       </c>
       <c r="H204">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J204" t="s">
         <v>55</v>
@@ -8546,13 +8546,13 @@
         <v>1</v>
       </c>
       <c r="F205">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G205" t="s">
         <v>252</v>
       </c>
       <c r="H205">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J205" t="s">
         <v>55</v>
@@ -8578,13 +8578,13 @@
         <v>1</v>
       </c>
       <c r="F206">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G206" t="s">
         <v>256</v>
       </c>
       <c r="H206">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J206" t="s">
         <v>55</v>
@@ -8610,10 +8610,10 @@
         <v>1</v>
       </c>
       <c r="F207">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H207">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J207" t="s">
         <v>55</v>
@@ -8639,13 +8639,13 @@
         <v>2</v>
       </c>
       <c r="F208">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G208" t="s">
         <v>330</v>
       </c>
       <c r="H208">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J208" t="s">
         <v>55</v>
@@ -8671,13 +8671,13 @@
         <v>1</v>
       </c>
       <c r="F209">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G209" t="s">
         <v>336</v>
       </c>
       <c r="H209">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J209" t="s">
         <v>55</v>
@@ -8703,13 +8703,13 @@
         <v>1</v>
       </c>
       <c r="F210">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G210" t="s">
         <v>247</v>
       </c>
       <c r="H210">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J210" t="s">
         <v>55</v>
@@ -8735,13 +8735,13 @@
         <v>1</v>
       </c>
       <c r="F211">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G211" t="s">
         <v>419</v>
       </c>
       <c r="H211">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J211" t="s">
         <v>55</v>
@@ -8767,13 +8767,13 @@
         <v>1</v>
       </c>
       <c r="F212">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G212" t="s">
         <v>115</v>
       </c>
       <c r="H212">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J212" t="s">
         <v>55</v>
@@ -8805,10 +8805,10 @@
         <v>1</v>
       </c>
       <c r="F213">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H213">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J213" t="s">
         <v>55</v>
@@ -8840,16 +8840,16 @@
         <v>1</v>
       </c>
       <c r="F214">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G214" t="s">
         <v>455</v>
       </c>
       <c r="H214">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I214">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J214" t="s">
         <v>55</v>
@@ -8878,13 +8878,13 @@
         <v>1</v>
       </c>
       <c r="F215">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G215" t="s">
         <v>469</v>
       </c>
       <c r="H215">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J215" t="s">
         <v>55</v>
@@ -8913,10 +8913,10 @@
         <v>1</v>
       </c>
       <c r="F216">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H216">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J216" t="s">
         <v>55</v>
@@ -8945,13 +8945,13 @@
         <v>1</v>
       </c>
       <c r="F217">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G217" t="s">
         <v>247</v>
       </c>
       <c r="H217">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J217" t="s">
         <v>55</v>
@@ -8977,13 +8977,13 @@
         <v>1</v>
       </c>
       <c r="F218">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G218" t="s">
         <v>478</v>
       </c>
       <c r="H218">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J218" t="s">
         <v>55</v>
@@ -9012,13 +9012,13 @@
         <v>1</v>
       </c>
       <c r="F219">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G219" t="s">
         <v>115</v>
       </c>
       <c r="H219">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J219" t="s">
         <v>55</v>
@@ -9047,10 +9047,10 @@
         <v>1</v>
       </c>
       <c r="F220">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H220">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J220" t="s">
         <v>55</v>
@@ -9079,13 +9079,13 @@
         <v>1</v>
       </c>
       <c r="F221">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G221" t="s">
         <v>494</v>
       </c>
       <c r="H221">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J221" t="s">
         <v>55</v>
@@ -9114,10 +9114,10 @@
         <v>1</v>
       </c>
       <c r="F222">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H222">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J222" t="s">
         <v>55</v>
@@ -9143,10 +9143,10 @@
         <v>1</v>
       </c>
       <c r="F223">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H223">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J223" t="s">
         <v>55</v>
@@ -9172,13 +9172,13 @@
         <v>1</v>
       </c>
       <c r="F224">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G224" t="s">
         <v>501</v>
       </c>
       <c r="H224">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J224" t="s">
         <v>55</v>
@@ -9207,10 +9207,10 @@
         <v>1</v>
       </c>
       <c r="F225">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H225">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J225" t="s">
         <v>55</v>
@@ -9239,10 +9239,10 @@
         <v>1</v>
       </c>
       <c r="F226">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H226">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J226" t="s">
         <v>55</v>
@@ -9271,10 +9271,10 @@
         <v>2</v>
       </c>
       <c r="F227">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H227">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J227" t="s">
         <v>55</v>
@@ -9303,10 +9303,10 @@
         <v>2</v>
       </c>
       <c r="F228">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H228">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J228" t="s">
         <v>55</v>
@@ -9335,10 +9335,10 @@
         <v>1</v>
       </c>
       <c r="F229">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H229">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J229" t="s">
         <v>55</v>
@@ -9367,10 +9367,10 @@
         <v>2</v>
       </c>
       <c r="F230">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H230">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J230" t="s">
         <v>55</v>
@@ -9399,10 +9399,10 @@
         <v>2</v>
       </c>
       <c r="F231">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H231">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J231" t="s">
         <v>55</v>
@@ -9431,10 +9431,10 @@
         <v>1</v>
       </c>
       <c r="F232">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H232">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J232" t="s">
         <v>55</v>
@@ -9463,13 +9463,13 @@
         <v>2</v>
       </c>
       <c r="F233">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H233">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I233">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="J233" t="s">
         <v>55</v>
@@ -9498,10 +9498,10 @@
         <v>1</v>
       </c>
       <c r="F234">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H234">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J234" t="s">
         <v>55</v>
@@ -9530,10 +9530,10 @@
         <v>1</v>
       </c>
       <c r="F235">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H235">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J235" t="s">
         <v>55</v>
@@ -9562,10 +9562,10 @@
         <v>1</v>
       </c>
       <c r="F236">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H236">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J236" t="s">
         <v>55</v>
@@ -9594,10 +9594,10 @@
         <v>1</v>
       </c>
       <c r="F237">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H237">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J237" t="s">
         <v>55</v>
@@ -9626,10 +9626,10 @@
         <v>1</v>
       </c>
       <c r="F238">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H238">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J238" t="s">
         <v>55</v>
@@ -9658,10 +9658,10 @@
         <v>1</v>
       </c>
       <c r="F239">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H239">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J239" t="s">
         <v>55</v>
@@ -9690,13 +9690,13 @@
         <v>1</v>
       </c>
       <c r="F240">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H240">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="I240">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="J240" t="s">
         <v>55</v>
@@ -9725,10 +9725,10 @@
         <v>2</v>
       </c>
       <c r="F241">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H241">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J241" t="s">
         <v>55</v>
@@ -9757,10 +9757,10 @@
         <v>1</v>
       </c>
       <c r="F242">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H242">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J242" t="s">
         <v>55</v>
@@ -9789,10 +9789,10 @@
         <v>1</v>
       </c>
       <c r="F243">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H243">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J243" t="s">
         <v>55</v>
@@ -9821,10 +9821,10 @@
         <v>1</v>
       </c>
       <c r="F244">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H244">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J244" t="s">
         <v>55</v>
@@ -9853,10 +9853,10 @@
         <v>1</v>
       </c>
       <c r="F245">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H245">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J245" t="s">
         <v>55</v>
@@ -9885,10 +9885,10 @@
         <v>1</v>
       </c>
       <c r="F246">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H246">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J246" t="s">
         <v>55</v>
@@ -9917,10 +9917,10 @@
         <v>2</v>
       </c>
       <c r="F247">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H247">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J247" t="s">
         <v>55</v>
@@ -9949,10 +9949,10 @@
         <v>1</v>
       </c>
       <c r="F248">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H248">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J248" t="s">
         <v>55</v>
@@ -9981,10 +9981,10 @@
         <v>1</v>
       </c>
       <c r="F249">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H249">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J249" t="s">
         <v>55</v>
@@ -10013,10 +10013,10 @@
         <v>1</v>
       </c>
       <c r="F250">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H250">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J250" t="s">
         <v>603</v>
@@ -10045,16 +10045,16 @@
         <v>1</v>
       </c>
       <c r="F251">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G251" t="s">
         <v>7</v>
       </c>
       <c r="H251">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I251">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J251" t="s">
         <v>8</v>
@@ -10083,13 +10083,13 @@
         <v>1</v>
       </c>
       <c r="F252">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G252" t="s">
         <v>11</v>
       </c>
       <c r="H252">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J252" t="s">
         <v>8</v>
@@ -10118,13 +10118,13 @@
         <v>1</v>
       </c>
       <c r="F253">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G253" t="s">
         <v>40</v>
       </c>
       <c r="H253">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J253" t="s">
         <v>8</v>
@@ -10153,10 +10153,10 @@
         <v>1</v>
       </c>
       <c r="F254">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H254">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J254" t="s">
         <v>8</v>
@@ -10182,13 +10182,13 @@
         <v>1</v>
       </c>
       <c r="F255">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G255" t="s">
         <v>107</v>
       </c>
       <c r="H255">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J255" t="s">
         <v>8</v>
@@ -10214,10 +10214,10 @@
         <v>1</v>
       </c>
       <c r="F256">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H256">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J256" t="s">
         <v>8</v>
@@ -10243,13 +10243,13 @@
         <v>1</v>
       </c>
       <c r="F257">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H257">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I257">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J257" t="s">
         <v>8</v>
@@ -10275,10 +10275,10 @@
         <v>1</v>
       </c>
       <c r="F258">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H258">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J258" t="s">
         <v>8</v>
@@ -10304,13 +10304,13 @@
         <v>1</v>
       </c>
       <c r="F259">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G259" t="s">
         <v>169</v>
       </c>
       <c r="H259">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J259" t="s">
         <v>8</v>
@@ -10336,10 +10336,10 @@
         <v>1</v>
       </c>
       <c r="F260">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H260">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J260" t="s">
         <v>8</v>
@@ -10365,10 +10365,10 @@
         <v>1</v>
       </c>
       <c r="F261">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H261">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J261" t="s">
         <v>8</v>
@@ -10394,10 +10394,10 @@
         <v>1</v>
       </c>
       <c r="F262">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H262">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J262" t="s">
         <v>8</v>
@@ -10423,13 +10423,13 @@
         <v>1</v>
       </c>
       <c r="F263">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G263" t="s">
         <v>424</v>
       </c>
       <c r="H263">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J263" t="s">
         <v>8</v>
@@ -10455,13 +10455,13 @@
         <v>1</v>
       </c>
       <c r="F264">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G264" t="s">
         <v>430</v>
       </c>
       <c r="H264">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J264" t="s">
         <v>8</v>
@@ -10487,13 +10487,13 @@
         <v>1</v>
       </c>
       <c r="F265">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G265" t="s">
         <v>466</v>
       </c>
       <c r="H265">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J265" t="s">
         <v>8</v>
@@ -10522,13 +10522,13 @@
         <v>1</v>
       </c>
       <c r="F266">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G266" t="s">
         <v>504</v>
       </c>
       <c r="H266">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J266" t="s">
         <v>8</v>
@@ -10557,10 +10557,10 @@
         <v>2</v>
       </c>
       <c r="F267">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H267">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J267" t="s">
         <v>8</v>
@@ -10589,13 +10589,13 @@
         <v>1</v>
       </c>
       <c r="F268">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G268" t="s">
         <v>524</v>
       </c>
       <c r="H268">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J268" t="s">
         <v>8</v>
@@ -10624,13 +10624,13 @@
         <v>1</v>
       </c>
       <c r="F269">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G269" t="s">
         <v>530</v>
       </c>
       <c r="H269">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J269" t="s">
         <v>8</v>
@@ -10659,13 +10659,13 @@
         <v>1</v>
       </c>
       <c r="F270">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G270" t="s">
         <v>548</v>
       </c>
       <c r="H270">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J270" t="s">
         <v>8</v>
@@ -10694,10 +10694,10 @@
         <v>1</v>
       </c>
       <c r="F271">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H271">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J271" t="s">
         <v>8</v>
@@ -10726,13 +10726,13 @@
         <v>1</v>
       </c>
       <c r="F272">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G272" t="s">
         <v>572</v>
       </c>
       <c r="H272">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J272" t="s">
         <v>8</v>
@@ -10761,10 +10761,10 @@
         <v>1</v>
       </c>
       <c r="F273">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H273">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J273" t="s">
         <v>8</v>
@@ -10793,10 +10793,10 @@
         <v>1</v>
       </c>
       <c r="F274">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H274">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J274" t="s">
         <v>8</v>
@@ -10825,10 +10825,10 @@
         <v>1</v>
       </c>
       <c r="F275">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H275">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J275" t="s">
         <v>8</v>
@@ -10857,10 +10857,10 @@
         <v>1</v>
       </c>
       <c r="F276">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H276">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J276" t="s">
         <v>8</v>
@@ -10889,10 +10889,10 @@
         <v>1</v>
       </c>
       <c r="F277">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H277">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J277" t="s">
         <v>545</v>
@@ -10921,13 +10921,13 @@
         <v>2</v>
       </c>
       <c r="F278">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G278" t="s">
         <v>3</v>
       </c>
       <c r="H278">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J278" t="s">
         <v>4</v>
@@ -10956,10 +10956,10 @@
         <v>1</v>
       </c>
       <c r="F279">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H279">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J279" t="s">
         <v>4</v>
@@ -10988,10 +10988,10 @@
         <v>1</v>
       </c>
       <c r="F280">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H280">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J280" t="s">
         <v>4</v>
@@ -11020,10 +11020,10 @@
         <v>1</v>
       </c>
       <c r="F281">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H281">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J281" t="s">
         <v>19</v>
@@ -11052,10 +11052,10 @@
         <v>1</v>
       </c>
       <c r="F282">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H282">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J282" t="s">
         <v>19</v>
@@ -11081,10 +11081,10 @@
         <v>1</v>
       </c>
       <c r="F283">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H283">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J283" t="s">
         <v>19</v>
@@ -11110,13 +11110,13 @@
         <v>1</v>
       </c>
       <c r="F284">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G284" t="s">
         <v>115</v>
       </c>
       <c r="H284">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J284" t="s">
         <v>19</v>
@@ -11142,10 +11142,10 @@
         <v>1</v>
       </c>
       <c r="F285">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H285">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J285" t="s">
         <v>19</v>
@@ -11171,10 +11171,10 @@
         <v>2</v>
       </c>
       <c r="F286">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H286">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J286" t="s">
         <v>19</v>
@@ -11200,10 +11200,10 @@
         <v>1</v>
       </c>
       <c r="F287">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H287">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J287" t="s">
         <v>19</v>
@@ -11229,10 +11229,10 @@
         <v>1</v>
       </c>
       <c r="F288">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H288">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J288" t="s">
         <v>19</v>
@@ -11258,10 +11258,10 @@
         <v>1</v>
       </c>
       <c r="F289">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H289">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J289" t="s">
         <v>19</v>
@@ -11287,13 +11287,13 @@
         <v>1</v>
       </c>
       <c r="F290">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G290" t="s">
         <v>381</v>
       </c>
       <c r="H290">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J290" t="s">
         <v>19</v>
@@ -11319,13 +11319,13 @@
         <v>1</v>
       </c>
       <c r="F291">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G291" t="s">
         <v>115</v>
       </c>
       <c r="H291">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J291" t="s">
         <v>19</v>
@@ -11354,10 +11354,10 @@
         <v>1</v>
       </c>
       <c r="F292">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H292">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J292" t="s">
         <v>19</v>
@@ -11389,10 +11389,10 @@
         <v>1</v>
       </c>
       <c r="F293">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H293">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J293" t="s">
         <v>19</v>
@@ -11421,10 +11421,10 @@
         <v>1</v>
       </c>
       <c r="F294">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H294">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J294" t="s">
         <v>19</v>
@@ -11453,10 +11453,10 @@
         <v>1</v>
       </c>
       <c r="F295">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H295">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J295" t="s">
         <v>19</v>
@@ -11485,10 +11485,10 @@
         <v>1</v>
       </c>
       <c r="F296">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H296">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J296" t="s">
         <v>19</v>
@@ -11517,10 +11517,10 @@
         <v>1</v>
       </c>
       <c r="F297">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H297">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J297" t="s">
         <v>19</v>
@@ -11549,10 +11549,10 @@
         <v>1</v>
       </c>
       <c r="F298">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H298">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J298" t="s">
         <v>19</v>
@@ -11581,10 +11581,10 @@
         <v>1</v>
       </c>
       <c r="F299">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H299">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J299" t="s">
         <v>201</v>
@@ -11610,10 +11610,10 @@
         <v>2</v>
       </c>
       <c r="F300">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H300">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J300" t="s">
         <v>201</v>
@@ -11639,13 +11639,13 @@
         <v>1</v>
       </c>
       <c r="F301">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G301" t="s">
         <v>208</v>
       </c>
       <c r="H301">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J301" t="s">
         <v>201</v>
@@ -11671,13 +11671,13 @@
         <v>1</v>
       </c>
       <c r="F302">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H302">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I302">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J302" t="s">
         <v>201</v>
@@ -11703,10 +11703,10 @@
         <v>1</v>
       </c>
       <c r="F303">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H303">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J303" t="s">
         <v>201</v>
@@ -11732,13 +11732,13 @@
         <v>1</v>
       </c>
       <c r="F304">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G304" t="s">
         <v>15</v>
       </c>
       <c r="H304">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J304" t="s">
         <v>16</v>
@@ -11767,10 +11767,10 @@
         <v>1</v>
       </c>
       <c r="F305">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H305">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J305" t="s">
         <v>16</v>
@@ -11799,10 +11799,10 @@
         <v>1</v>
       </c>
       <c r="F306">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H306">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J306" t="s">
         <v>16</v>
@@ -11831,16 +11831,16 @@
         <v>1</v>
       </c>
       <c r="F307">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G307" t="s">
         <v>198</v>
       </c>
       <c r="H307">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I307">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J307" t="s">
         <v>16</v>
@@ -11866,10 +11866,10 @@
         <v>1</v>
       </c>
       <c r="F308">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H308">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J308" t="s">
         <v>16</v>
@@ -11895,10 +11895,10 @@
         <v>1</v>
       </c>
       <c r="F309">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H309">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="J309" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
feat(clients): complete client edit form with all fields
- Updated ClientsController edit method to load all dropdown options
- Completely rewrote clients/edit.blade.php to match create form structure
- Added all missing fields: cash_or_probono, status, dates, contact_lawyer, logo, document locations
- Added current logo preview in edit form
- Added missing translation keys for update_client and current_logo
- Form now includes proper validation and error handling

DoD: Client edit form now has all fields like create and view forms
</commit_message>
<xml_diff>
--- a/Access_Data_Export/clients.xlsx
+++ b/Access_Data_Export/clients.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Claude\Litigation_Database_Ver2\Litigation_Database_Ver2\Access_Data_Export\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F164B705-E121-4706-8FB2-2DA1F18F4EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BEC4DE2-2448-4809-B49C-3B59436F4518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2425,8 +2425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M309"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+    <sheetView tabSelected="1" topLeftCell="A178" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B214" sqref="B214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>